<commit_message>
q2: systematic factor analysis (bivariate)
</commit_message>
<xml_diff>
--- a/cmp/py/main/factors.xlsx
+++ b/cmp/py/main/factors.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yiqia\OneDrive\Documents\TeX\The-M3C\cmp\py\main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eba6016013cd6a40/Documents/TeX/The-M3C/cmp/py/main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1824C128-0EEE-46F9-A736-FA5D84758D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="13_ncr:1_{1824C128-0EEE-46F9-A736-FA5D84758D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82B16B51-0B94-4710-A5D5-B06DEA694F94}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{0E1049F4-1AF9-4A88-B449-DA03FF1D9724}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{0E1049F4-1AF9-4A88-B449-DA03FF1D9724}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>year</t>
   </si>
@@ -55,13 +55,22 @@
   <si>
     <t>gas_price</t>
   </si>
+  <si>
+    <t>env_perc</t>
+  </si>
+  <si>
+    <t>disp_inc</t>
+  </si>
+  <si>
+    <t>death_rate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -107,8 +116,8 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,18 +432,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3540A7EB-0300-4678-B263-6EDFAACAA532}">
-  <dimension ref="A1:R25"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -453,8 +463,17 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>2000</v>
       </c>
@@ -464,8 +483,14 @@
       <c r="E2">
         <v>58892514</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="H2">
+        <v>23112</v>
+      </c>
+      <c r="I2">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2001</v>
       </c>
@@ -475,8 +500,14 @@
       <c r="E3">
         <v>59119673</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="H3">
+        <v>23716</v>
+      </c>
+      <c r="I3">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>2002</v>
       </c>
@@ -486,8 +517,14 @@
       <c r="E4">
         <v>59370479</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="H4">
+        <v>24296</v>
+      </c>
+      <c r="I4">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>2003</v>
       </c>
@@ -500,8 +537,17 @@
       <c r="F5" s="2">
         <v>77.287332733333344</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>24999</v>
+      </c>
+      <c r="I5" s="1">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>2004</v>
       </c>
@@ -514,8 +560,17 @@
       <c r="F6" s="2">
         <v>81.89400307692307</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>25404</v>
+      </c>
+      <c r="I6" s="1">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>2005</v>
       </c>
@@ -528,8 +583,17 @@
       <c r="F7" s="2">
         <v>90.820265769230801</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="G7" s="1">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>25978</v>
+      </c>
+      <c r="I7" s="1">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>2006</v>
       </c>
@@ -539,27 +603,33 @@
       <c r="C8" s="7">
         <v>9.3389980000000001</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
       <c r="E8" s="1">
         <v>60846820</v>
       </c>
       <c r="F8" s="3">
         <v>95.179094230769209</v>
       </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="G8" s="1">
+        <v>3</v>
+      </c>
+      <c r="H8" s="1">
+        <v>26088</v>
+      </c>
+      <c r="I8" s="1">
+        <v>395</v>
+      </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>2007</v>
       </c>
@@ -569,27 +639,33 @@
       <c r="C9" s="7">
         <v>9.1341870000000007</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
       <c r="E9" s="1">
         <v>61322463</v>
       </c>
       <c r="F9" s="3">
         <v>97.112431773584888</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="G9" s="1">
+        <v>3</v>
+      </c>
+      <c r="H9" s="1">
+        <v>26167</v>
+      </c>
+      <c r="I9" s="1">
+        <v>381</v>
+      </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>2008</v>
       </c>
@@ -599,27 +675,33 @@
       <c r="C10" s="7">
         <v>8.8259380000000007</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1">
+        <v>34</v>
+      </c>
       <c r="E10" s="1">
         <v>61806995</v>
       </c>
       <c r="F10" s="3">
         <v>117.55670228846155</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="G10" s="1">
+        <v>4</v>
+      </c>
+      <c r="H10" s="1">
+        <v>25460</v>
+      </c>
+      <c r="I10" s="1">
+        <v>372</v>
+      </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>2009</v>
       </c>
@@ -629,27 +711,33 @@
       <c r="C11" s="7">
         <v>7.9383169999999996</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1">
+        <v>100</v>
+      </c>
       <c r="E11" s="1">
         <v>62276270</v>
       </c>
       <c r="F11" s="3">
         <v>104.14661392307693</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="G11" s="1">
+        <v>5</v>
+      </c>
+      <c r="H11" s="1">
+        <v>24180</v>
+      </c>
+      <c r="I11" s="1">
+        <v>346</v>
+      </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>2010</v>
       </c>
@@ -668,20 +756,24 @@
       <c r="F12" s="3">
         <v>119.23461471153846</v>
       </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="G12" s="1">
+        <v>6</v>
+      </c>
+      <c r="H12" s="1">
+        <v>24758</v>
+      </c>
+      <c r="I12" s="1">
+        <v>336</v>
+      </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>2011</v>
       </c>
@@ -700,20 +792,24 @@
       <c r="F13" s="3">
         <v>138.80538244230769</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="G13" s="1">
+        <v>7</v>
+      </c>
+      <c r="H13" s="1">
+        <v>24856</v>
+      </c>
+      <c r="I13" s="1">
+        <v>309</v>
+      </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>2012</v>
       </c>
@@ -732,20 +828,24 @@
       <c r="F14" s="3">
         <v>142.16340853122639</v>
       </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+      <c r="G14" s="1">
+        <v>7</v>
+      </c>
+      <c r="H14" s="1">
+        <v>24711</v>
+      </c>
+      <c r="I14" s="1">
+        <v>305</v>
+      </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>2013</v>
       </c>
@@ -764,20 +864,24 @@
       <c r="F15" s="3">
         <v>140.58729698076925</v>
       </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="G15" s="1">
+        <v>7</v>
+      </c>
+      <c r="H15" s="1">
+        <v>24863</v>
+      </c>
+      <c r="I15" s="1">
+        <v>298</v>
+      </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>2014</v>
       </c>
@@ -796,20 +900,24 @@
       <c r="F16" s="3">
         <v>133.47403719539324</v>
       </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+      <c r="G16" s="1">
+        <v>10</v>
+      </c>
+      <c r="H16" s="1">
+        <v>25591</v>
+      </c>
+      <c r="I16" s="1">
+        <v>284</v>
+      </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>2015</v>
       </c>
@@ -828,20 +936,24 @@
       <c r="F17" s="3">
         <v>114.99686980524916</v>
       </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+      <c r="G17" s="1">
+        <v>9</v>
+      </c>
+      <c r="H17" s="1">
+        <v>26098</v>
+      </c>
+      <c r="I17" s="1">
+        <v>290</v>
+      </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>2016</v>
       </c>
@@ -860,20 +972,24 @@
       <c r="F18" s="3">
         <v>110.42004491107694</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="G18" s="1">
+        <v>9</v>
+      </c>
+      <c r="H18" s="1">
+        <v>26392</v>
+      </c>
+      <c r="I18" s="1">
+        <v>276</v>
+      </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>2017</v>
       </c>
@@ -892,20 +1008,24 @@
       <c r="F19" s="3">
         <v>120.20657375815381</v>
       </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
+      <c r="G19" s="1">
+        <v>9</v>
+      </c>
+      <c r="H19" s="1">
+        <v>27192</v>
+      </c>
+      <c r="I19" s="1">
+        <v>272</v>
+      </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>2018</v>
       </c>
@@ -924,20 +1044,24 @@
       <c r="F20" s="3">
         <v>130.03552002581134</v>
       </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
+      <c r="G20" s="1">
+        <v>13</v>
+      </c>
+      <c r="H20" s="1">
+        <v>27334</v>
+      </c>
+      <c r="I20" s="1">
+        <v>266</v>
+      </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>2019</v>
       </c>
@@ -956,24 +1080,30 @@
       <c r="F21" s="3">
         <v>131.70777434969222</v>
       </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
+      <c r="G21" s="1">
+        <v>25</v>
+      </c>
+      <c r="H21" s="1">
+        <v>28118</v>
+      </c>
+      <c r="I21" s="1">
+        <v>254</v>
+      </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>2020</v>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22" s="1">
+        <v>4184</v>
+      </c>
       <c r="C22" s="7">
         <v>4.8652816000000003</v>
       </c>
@@ -986,24 +1116,30 @@
       <c r="F22" s="3">
         <v>119.45585764984614</v>
       </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
+      <c r="G22" s="1">
+        <v>25</v>
+      </c>
+      <c r="H22" s="1">
+        <v>23750</v>
+      </c>
+      <c r="I22" s="1">
+        <v>259</v>
+      </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>2021</v>
       </c>
-      <c r="B23" s="1"/>
+      <c r="B23" s="1">
+        <v>4849</v>
+      </c>
       <c r="C23" s="7">
         <v>5.1540995000000001</v>
       </c>
@@ -1016,20 +1152,24 @@
       <c r="F23" s="3">
         <v>135.03788687656407</v>
       </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
+      <c r="G23" s="1">
+        <v>30</v>
+      </c>
+      <c r="H23" s="1">
+        <v>26589</v>
+      </c>
+      <c r="I23" s="1">
+        <v>260</v>
+      </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>2022</v>
       </c>
@@ -1037,8 +1177,11 @@
       <c r="F24" s="2">
         <v>177.7783726923077</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="G24">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>2023</v>
       </c>
@@ -1048,6 +1191,11 @@
       </c>
     </row>
   </sheetData>
+  <dataConsolidate function="average" leftLabels="1">
+    <dataRefs count="1">
+      <dataRef ref="M8:N1037" sheet="Sheet1"/>
+    </dataRefs>
+  </dataConsolidate>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>